<commit_message>
update AndroidTraining and CheckList
</commit_message>
<xml_diff>
--- a/docs/CheckList.xlsx
+++ b/docs/CheckList.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
   <si>
     <t>Android Training (1 week : 20/8 →26/8 – 5 days)
 27/8: review</t>
@@ -45,7 +45,7 @@
     <t>2-3h</t>
   </si>
   <si>
-    <t>20/8</t>
+    <t>Chốt 24/8 xong</t>
   </si>
   <si>
     <t>Activity, lauch mode
@@ -61,9 +61,6 @@
     <t>Các loại service, dùng khi nào</t>
   </si>
   <si>
-    <t>21/8</t>
-  </si>
-  <si>
     <t>Thread, AsysTask</t>
   </si>
   <si>
@@ -77,9 +74,6 @@
   </si>
   <si>
     <t>SQLite</t>
-  </si>
-  <si>
-    <t>24/8</t>
   </si>
   <si>
     <t>Animation</t>
@@ -174,6 +168,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -194,22 +189,26 @@
       <sz val="24"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="20"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="20"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="14"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -279,16 +278,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -308,19 +307,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -411,7 +406,9 @@
   <cols>
     <col collapsed="false" hidden="false" max="14" min="1" style="0" width="11.5204081632653"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="18.9897959183673"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -658,16 +655,14 @@
       </c>
       <c r="O16" s="6"/>
       <c r="P16" s="5"/>
-      <c r="Q16" s="8" t="s">
-        <v>14</v>
-      </c>
+      <c r="Q16" s="7"/>
     </row>
     <row r="17" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B17" s="5" t="n">
         <v>5</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
@@ -684,14 +679,14 @@
       </c>
       <c r="O17" s="6"/>
       <c r="P17" s="5"/>
-      <c r="Q17" s="8"/>
+      <c r="Q17" s="7"/>
     </row>
     <row r="18" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B18" s="5" t="n">
         <v>6</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
@@ -708,21 +703,21 @@
       </c>
       <c r="O18" s="6"/>
       <c r="P18" s="5"/>
-      <c r="Q18" s="8"/>
+      <c r="Q18" s="7"/>
     </row>
     <row r="19" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B19" s="5" t="n">
         <v>7</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
       <c r="H19" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
@@ -734,14 +729,14 @@
       </c>
       <c r="O19" s="6"/>
       <c r="P19" s="5"/>
-      <c r="Q19" s="8"/>
+      <c r="Q19" s="7"/>
     </row>
     <row r="20" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B20" s="5" t="n">
         <v>8</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
@@ -758,16 +753,14 @@
       </c>
       <c r="O20" s="6"/>
       <c r="P20" s="5"/>
-      <c r="Q20" s="8" t="s">
-        <v>20</v>
-      </c>
+      <c r="Q20" s="7"/>
     </row>
     <row r="21" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B21" s="5" t="n">
         <v>9</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
@@ -784,19 +777,19 @@
       </c>
       <c r="O21" s="6"/>
       <c r="P21" s="5"/>
-      <c r="Q21" s="8"/>
-      <c r="R21" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="S21" s="9"/>
-      <c r="T21" s="9"/>
+      <c r="Q21" s="7"/>
+      <c r="R21" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="S21" s="8"/>
+      <c r="T21" s="8"/>
     </row>
     <row r="22" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B22" s="5" t="n">
         <v>10</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
@@ -813,10 +806,10 @@
       </c>
       <c r="O22" s="6"/>
       <c r="P22" s="5"/>
-      <c r="Q22" s="8"/>
-      <c r="R22" s="9"/>
-      <c r="S22" s="9"/>
-      <c r="T22" s="9"/>
+      <c r="Q22" s="7"/>
+      <c r="R22" s="8"/>
+      <c r="S22" s="8"/>
+      <c r="T22" s="8"/>
     </row>
     <row r="23" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B23" s="5" t="n">
@@ -876,21 +869,21 @@
       <c r="P25" s="5"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B41" s="10"/>
-      <c r="C41" s="10"/>
-      <c r="D41" s="10"/>
-      <c r="E41" s="10"/>
-      <c r="F41" s="10"/>
-      <c r="G41" s="10"/>
-      <c r="H41" s="10"/>
-      <c r="I41" s="10"/>
+      <c r="A41" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B41" s="9"/>
+      <c r="C41" s="9"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9"/>
+      <c r="G41" s="9"/>
+      <c r="H41" s="9"/>
+      <c r="I41" s="9"/>
     </row>
     <row r="62" customFormat="false" ht="578.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="49">
+  <mergeCells count="47">
     <mergeCell ref="B4:S8"/>
     <mergeCell ref="L10:S10"/>
     <mergeCell ref="C12:G12"/>
@@ -899,7 +892,7 @@
     <mergeCell ref="C13:G13"/>
     <mergeCell ref="H13:M13"/>
     <mergeCell ref="N13:O13"/>
-    <mergeCell ref="Q13:Q15"/>
+    <mergeCell ref="Q13:Q22"/>
     <mergeCell ref="C14:G14"/>
     <mergeCell ref="H14:M14"/>
     <mergeCell ref="N14:O14"/>
@@ -909,7 +902,6 @@
     <mergeCell ref="C16:G16"/>
     <mergeCell ref="H16:M16"/>
     <mergeCell ref="N16:O16"/>
-    <mergeCell ref="Q16:Q19"/>
     <mergeCell ref="C17:G17"/>
     <mergeCell ref="H17:M17"/>
     <mergeCell ref="N17:O17"/>
@@ -922,7 +914,6 @@
     <mergeCell ref="C20:G20"/>
     <mergeCell ref="H20:M20"/>
     <mergeCell ref="N20:O20"/>
-    <mergeCell ref="Q20:Q22"/>
     <mergeCell ref="C21:G21"/>
     <mergeCell ref="H21:M21"/>
     <mergeCell ref="N21:O21"/>

</xml_diff>

<commit_message>
update AndroidTraining.docx and CheckList.xlsx
</commit_message>
<xml_diff>
--- a/docs/CheckList.xlsx
+++ b/docs/CheckList.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Research " sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Coding" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
@@ -211,7 +212,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -236,6 +237,12 @@
         <bgColor rgb="FF33CCCC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF6600"/>
+        <bgColor rgb="FFFF9900"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
@@ -278,7 +285,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -308,6 +315,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -398,8 +413,8 @@
   </sheetPr>
   <dimension ref="A4:T62"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q13" activeCellId="0" sqref="Q13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A41" activeCellId="0" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -632,53 +647,53 @@
       <c r="Q15" s="7"/>
     </row>
     <row r="16" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B16" s="5" t="n">
+      <c r="B16" s="8" t="n">
         <v>4</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="5" t="s">
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="5"/>
-      <c r="N16" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="O16" s="6"/>
-      <c r="P16" s="5"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="O16" s="9"/>
+      <c r="P16" s="8"/>
       <c r="Q16" s="7"/>
     </row>
     <row r="17" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B17" s="5" t="n">
+      <c r="B17" s="8" t="n">
         <v>5</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
-      <c r="N17" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="O17" s="6"/>
-      <c r="P17" s="5"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="O17" s="9"/>
+      <c r="P17" s="8"/>
       <c r="Q17" s="7"/>
     </row>
     <row r="18" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -732,27 +747,27 @@
       <c r="Q19" s="7"/>
     </row>
     <row r="20" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B20" s="5" t="n">
-        <v>8</v>
-      </c>
-      <c r="C20" s="6" t="s">
+      <c r="B20" s="8" t="n">
+        <v>8</v>
+      </c>
+      <c r="C20" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="5"/>
-      <c r="N20" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="O20" s="6"/>
-      <c r="P20" s="5"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="O20" s="9"/>
+      <c r="P20" s="8"/>
       <c r="Q20" s="7"/>
     </row>
     <row r="21" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -778,11 +793,11 @@
       <c r="O21" s="6"/>
       <c r="P21" s="5"/>
       <c r="Q21" s="7"/>
-      <c r="R21" s="8" t="s">
+      <c r="R21" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="S21" s="8"/>
-      <c r="T21" s="8"/>
+      <c r="S21" s="10"/>
+      <c r="T21" s="10"/>
     </row>
     <row r="22" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B22" s="5" t="n">
@@ -807,9 +822,9 @@
       <c r="O22" s="6"/>
       <c r="P22" s="5"/>
       <c r="Q22" s="7"/>
-      <c r="R22" s="8"/>
-      <c r="S22" s="8"/>
-      <c r="T22" s="8"/>
+      <c r="R22" s="10"/>
+      <c r="S22" s="10"/>
+      <c r="T22" s="10"/>
     </row>
     <row r="23" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B23" s="5" t="n">
@@ -869,17 +884,17 @@
       <c r="P25" s="5"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="9" t="s">
+      <c r="A41" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B41" s="9"/>
-      <c r="C41" s="9"/>
-      <c r="D41" s="9"/>
-      <c r="E41" s="9"/>
-      <c r="F41" s="9"/>
-      <c r="G41" s="9"/>
-      <c r="H41" s="9"/>
-      <c r="I41" s="9"/>
+      <c r="B41" s="11"/>
+      <c r="C41" s="11"/>
+      <c r="D41" s="11"/>
+      <c r="E41" s="11"/>
+      <c r="F41" s="11"/>
+      <c r="G41" s="11"/>
+      <c r="H41" s="11"/>
+      <c r="I41" s="11"/>
     </row>
     <row r="62" customFormat="false" ht="578.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -940,4 +955,30 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>